<commit_message>
update readme.  Add 2nd wireframe, update spreadsheet
</commit_message>
<xml_diff>
--- a/planning/favorite-team-bkend.xlsx
+++ b/planning/favorite-team-bkend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx37112/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94709FF3-D148-6045-A5D9-4556D6E08CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C83AF63-8CDA-EF4D-AC6D-7EF09F464E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="3360" windowWidth="19080" windowHeight="15580" activeTab="2" xr2:uid="{30F2F74D-3599-DD4E-851F-DEEBE6535F10}"/>
+    <workbookView xWindow="3680" yWindow="3800" windowWidth="19080" windowHeight="15580" xr2:uid="{30F2F74D-3599-DD4E-851F-DEEBE6535F10}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="67">
   <si>
     <t>TABLES:</t>
   </si>
@@ -125,9 +125,6 @@
     <t>As a team fan I want a way to add players to the team</t>
   </si>
   <si>
-    <t>as a sports fan I want to see deatails about a player</t>
-  </si>
-  <si>
     <t>char</t>
   </si>
   <si>
@@ -225,6 +222,21 @@
   </si>
   <si>
     <t>tackles</t>
+  </si>
+  <si>
+    <t>Could add a Player Detail page which shows some additonal stats about the player</t>
+  </si>
+  <si>
+    <t>Possible future additions:</t>
+  </si>
+  <si>
+    <t>SportDetails table to hold stats by sport and position.  It would be used to get stats that fit the players sport and positon.  For example, ERA, W, L for pitchers and BA, HR, RBI for position players.</t>
+  </si>
+  <si>
+    <t>API call to get current player stats</t>
+  </si>
+  <si>
+    <t>ability to update team or player once it is created</t>
   </si>
 </sst>
 </file>
@@ -593,11 +605,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156BD94D-E75B-6F44-B627-652FF97FA6C3}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -624,11 +634,6 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -641,11 +646,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6392E4F5-6407-0C42-8F6A-D4D42E6AFFD3}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -749,7 +752,7 @@
         <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -772,7 +775,7 @@
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -789,7 +792,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -799,6 +802,9 @@
       <c r="J8" t="s">
         <v>6</v>
       </c>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -816,33 +822,28 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
+      <c r="A14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -857,9 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E09289-6D82-024E-A5E4-FB8EF26641CF}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -924,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -932,12 +931,12 @@
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>11</v>
@@ -953,7 +952,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -971,7 +970,7 @@
         <v>12</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
@@ -984,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -996,7 +995,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
@@ -1009,7 +1008,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1052,7 +1051,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1076,16 +1075,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1101,16 +1100,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1153,7 +1152,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1173,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -1194,7 +1193,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -1215,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
@@ -1236,7 +1235,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
@@ -1257,7 +1256,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2">
         <v>2</v>
@@ -1313,19 +1312,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1342,19 +1341,19 @@
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1415,19 +1414,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1442,19 +1441,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1469,19 +1468,19 @@
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>

</xml_diff>